<commit_message>
Update mig_stoch_crm function with new argument structure
</commit_message>
<xml_diff>
--- a/data-raw/mCRM_bird_parameter_Defaults.xlsx
+++ b/data-raw/mCRM_bird_parameter_Defaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\PROJECTS_CURRENT\HC0054 - MSS update to sCRM\300 - Technical\mCRM\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HC0054 - MSS update to sCRM\300 - Technical\mCRM\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7709148E-150A-4EF8-8F44-A1471EF0BD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D208196-378F-4A33-919A-11C14FDD2E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C3AA158-F65C-4955-A6B9-80286CA44754}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C3AA158-F65C-4955-A6B9-80286CA44754}"/>
   </bookViews>
   <sheets>
     <sheet name="Default Values" sheetId="1" r:id="rId1"/>
@@ -1285,37 +1285,37 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>0.876</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>6.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>87</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -5476,13 +5476,13 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>214</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>215</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>234</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>235</v>
       </c>
@@ -5642,10 +5642,10 @@
         <v>237</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
   </sheetData>

</xml_diff>